<commit_message>
project demo with stakeholder
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,6 +8,11 @@
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="TAG2" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="TAG3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="TAG4" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="TAG5" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="TAG6" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +418,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,7 +454,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>TAG1</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>0.00s</t>
@@ -468,6 +477,643 @@
       <c r="E2" t="inlineStr">
         <is>
           <t>0/0</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>TAG2</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.96s</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.96s</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>TAG3</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.11s</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1.11s</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TAG4</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>4.87s</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>4.87s</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>TAG5</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.41s</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1.41s</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>TAG6</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>1.29s</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>4/5</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1.29s</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>4/5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Trial</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Reaction Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('folder_1', 'ball_1 - Copy')</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1.09s</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('folder_1', 'ball_1')</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.78s</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('folder_2', 'ball_2')</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.57s</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('folder_3', 'ball_3')</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.20s</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('folder_4', 'ball_4')</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0.91s</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Trial</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Reaction Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('folder_1', 'ball_1')</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>17.61s</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('folder_1', 'ball_1 - Copy')</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2.83s</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('folder_2', 'ball_2')</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.56s</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('folder_3', 'ball_3')</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.03s</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('folder_4', 'ball_4')</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.33s</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Trial</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Reaction Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1')</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1.01s</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1 - Copy')</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1.93s</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('folder_2', 'ball_2')</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0.70s</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('folder_3', 'ball_3')</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.73s</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('folder_4', 'ball_4')</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.69s</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Trial</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Reaction Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('folder_3', 'ball_3')</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2.28s</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('folder_2', 'ball_2')</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2.06s</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('folder_4', 'ball_4')</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0.88s</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1 - Copy')</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.24s</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1')</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0.00s</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>incorrect</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
working on adding 2 option trials
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" state="visible" r:id="rId1"/>
@@ -13,6 +13,8 @@
     <sheet name="TAG4" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="TAG5" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="TAG6" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="TAG7" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="TAG8" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -49,15 +51,15 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -418,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,8 +617,62 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>TAG7</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>2.06s</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2.06s</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>TAG8</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>1.98s</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1.98s</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -634,7 +690,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -755,7 +811,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -876,7 +932,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -997,7 +1053,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1118,6 +1174,248 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Trial</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Reaction Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('folder_4', 'ball_4')</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2.51s</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1 - Copy')</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2.03s</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('folder_2', 'ball_2')</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.98s</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1')</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.91s</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('folder_3', 'ball_3')</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.88s</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Trial</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Reaction Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1 - Copy')</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2.81s</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('folder_3', 'ball_3')</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>2.11s</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1')</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>2.03s</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('folder_2', 'ball_2')</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.08s</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('folder_4', 'ball_4')</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.87s</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
restructured code for multiple trial options
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -15,6 +15,9 @@
     <sheet name="TAG6" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="TAG7" sheetId="7" state="visible" r:id="rId7"/>
     <sheet name="TAG8" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="TAG9" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="TAG10" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="TAG12" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -420,7 +423,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -668,6 +671,356 @@
       <c r="E9" t="inlineStr">
         <is>
           <t>5/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>TAG9</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>2.21s</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>2.21s</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>TAG10</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>0.78s</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>0.78s</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>5/5</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>TAG</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>0.00s</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>0.00s</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>0/0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>TAG12</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0.68s</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0.68s</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>2/5</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Trial</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Reaction Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('folder_3', 'ball_3')</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1.96s</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1')</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.63s</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('folder_4', 'ball_4')</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0.43s</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1 - Copy')</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0.40s</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('folder_2', 'ball_2')</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0.46s</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Trial</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Reaction Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('folder_3', 'ball_3')</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>2.03s</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('folder_4', 'ball_4')</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.82s</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('folder_2', 'ball_2')</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>0.00s</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1 - Copy')</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>0.00s</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>incorrect</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1')</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0.56s</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
         </is>
       </c>
     </row>
@@ -1418,4 +1771,125 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Trial</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Reaction Time</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>('folder_3', 'ball_3')</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>3.28s</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1 - Copy')</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>1.94s</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>('folder_4', 'ball_4')</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>1.95s</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>('atest', 'ball_1')</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>1.90s</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>('folder_2', 'ball_2')</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>1.96s</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>correct</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>